<commit_message>
updated heave decay but results still look bad
</commit_message>
<xml_diff>
--- a/experimental_runs/1_freeDecay/heaveDecay/heaveDecayCases.xlsx
+++ b/experimental_runs/1_freeDecay/heaveDecay/heaveDecayCases.xlsx
@@ -36,7 +36,7 @@
     <t>'squares.initDisp.initLinDisp(3)'</t>
   </si>
   <si>
-    <t>m</t>
+    <t>heaveDecay</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="29.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -422,28 +422,22 @@
         <v>0.03</v>
       </c>
       <c r="B3" s="1">
-        <f>-0.04394+$A$3</f>
-        <v>-1.3940000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="C3" s="1">
-        <f>-0.04394+$A$3</f>
-        <v>-1.3940000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="C3:G3" si="0">-0.04394+$A$3</f>
-        <v>-1.3940000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.3940000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.3940000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.3940000000000001E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -451,28 +445,22 @@
         <v>0.05</v>
       </c>
       <c r="B4" s="1">
-        <f>-0.04394+$A$4</f>
-        <v>6.0600000000000029E-3</v>
+        <v>0.05</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:G4" si="1">-0.04394+$A$4</f>
-        <v>6.0600000000000029E-3</v>
+        <v>0.05</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="1"/>
-        <v>6.0600000000000029E-3</v>
+        <v>0.05</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="1"/>
-        <v>6.0600000000000029E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="1"/>
-        <v>6.0600000000000029E-3</v>
+        <v>0.05</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>6.0600000000000029E-3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -480,28 +468,22 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B5" s="1">
-        <f>-0.04394+$A$5</f>
-        <v>2.6060000000000007E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:G5" si="2">-0.04394+$A$5</f>
-        <v>2.6060000000000007E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="2"/>
-        <v>2.6060000000000007E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="2"/>
-        <v>2.6060000000000007E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="2"/>
-        <v>2.6060000000000007E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="2"/>
-        <v>2.6060000000000007E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -509,28 +491,22 @@
         <v>0.1</v>
       </c>
       <c r="B6" s="1">
-        <f>-0.04394+$A$6</f>
-        <v>5.6060000000000006E-2</v>
+        <v>0.1</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:G6" si="3">-0.04394+$A$6</f>
-        <v>5.6060000000000006E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="3"/>
-        <v>5.6060000000000006E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="3"/>
-        <v>5.6060000000000006E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="3"/>
-        <v>5.6060000000000006E-2</v>
+        <v>0.1</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="3"/>
-        <v>5.6060000000000006E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -538,28 +514,22 @@
         <v>0.15</v>
       </c>
       <c r="B7" s="1">
-        <f>-0.04394+$A$7</f>
-        <v>0.10605999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7:G7" si="4">-0.04394+$A$7</f>
-        <v>0.10605999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="4"/>
-        <v>0.10605999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="4"/>
-        <v>0.10605999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="4"/>
-        <v>0.10605999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="4"/>
-        <v>0.10605999999999999</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2015b - reran heaveDecay with damping, looks better
</commit_message>
<xml_diff>
--- a/experimental_runs/1_freeDecay/heaveDecay/heaveDecayCases.xlsx
+++ b/experimental_runs/1_freeDecay/heaveDecay/heaveDecayCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="7485"/>
+    <workbookView xWindow="360" yWindow="140" windowWidth="14360" windowHeight="7490"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,15 +52,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -68,13 +74,229 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -378,157 +600,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G7"/>
+  <dimension ref="B1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G7"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="29.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3" s="12">
         <v>0.03</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="6">
         <v>0.03</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="2">
         <v>0.03</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="2">
         <v>0.03</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="2">
         <v>0.03</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="2">
         <v>0.03</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="7">
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="12">
         <v>0.05</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="6">
         <v>0.05</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="2">
         <v>0.05</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="2">
         <v>0.05</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="2">
         <v>0.05</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="2">
         <v>0.05</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="7">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="12">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="12">
         <v>0.1</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="6">
         <v>0.1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="2">
         <v>0.1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="2">
         <v>0.1</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="2">
         <v>0.1</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="2">
         <v>0.1</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="7">
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="13">
         <v>0.15</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="8">
         <v>0.15</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="9">
         <v>0.15</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="9">
         <v>0.15</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="9">
         <v>0.15</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="9">
         <v>0.15</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="10">
         <v>0.15</v>
       </c>
     </row>
@@ -544,7 +768,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -556,7 +780,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>